<commit_message>
Falta melhorar os teste utilizando AmazonForest
</commit_message>
<xml_diff>
--- a/Pos_Qualys/TabelasMSC-VictorBeltrao.xlsx
+++ b/Pos_Qualys/TabelasMSC-VictorBeltrao.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20408"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3350588\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DS\tsc_box\Pos_Qualys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CCC935-F2F1-4F90-B8F3-28271A9B9D97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6BEE103-EFD5-45FE-B6DE-772088BD5D69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{6E1B9671-647E-4367-A572-0BBB2E44E843}"/>
   </bookViews>
@@ -1442,8 +1442,8 @@
   </sheetPr>
   <dimension ref="B1:U99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C72" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="K92" sqref="K92"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52:F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>